<commit_message>
filter date v1 , removed unnecessary filters
</commit_message>
<xml_diff>
--- a/Data/DataSheet.xlsx
+++ b/Data/DataSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
   <si>
     <t>Actions</t>
   </si>
@@ -44,13 +44,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Generate Yearly Report for Vendor</t>
+    <t>Open</t>
   </si>
   <si>
-    <t>WI4</t>
+    <t>Research Client Check Copy</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>WI2</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,206 +397,478 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>809944</v>
+        <v>647572</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1">
-        <v>43232</v>
+        <v>42788</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>619534</v>
+        <v>587242</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1">
-        <v>43143</v>
+        <v>43063</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>532044</v>
+        <v>962522</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1">
-        <v>42903</v>
+        <v>43441</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>612294</v>
+        <v>612812</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1">
-        <v>42895</v>
+        <v>43075</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>640094</v>
+        <v>837862</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1">
-        <v>42996</v>
+        <v>43242</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>655994</v>
+        <v>906912</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1">
-        <v>43171</v>
+        <v>43381</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>640314</v>
+        <v>490572</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
-        <v>43294</v>
+        <v>43077</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>637964</v>
+        <v>295372</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
-        <v>43227</v>
+        <v>43051</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>193134</v>
+        <v>515842</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1">
-        <v>43193</v>
+        <v>43536</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>798064</v>
+        <v>699802</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1">
-        <v>42913</v>
+        <v>42888</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>442854</v>
+        <v>251502</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1">
-        <v>42995</v>
+        <v>43064</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>563864</v>
+        <v>321742</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13" s="1">
-        <v>43483</v>
+        <v>42823</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>239522</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1">
+        <v>43004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>802782</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1">
+        <v>43150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>636492</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <v>43516</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>697552</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1">
+        <v>43231</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>760052</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1">
+        <v>42896</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>191382</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>43141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>479542</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>758992</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>746282</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1">
+        <v>43188</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>562152</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1">
+        <v>42867</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>436842</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1">
+        <v>42803</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>583912</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>367012</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="1">
+        <v>43319</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>982202</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1">
+        <v>42774</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>419692</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1">
+        <v>43455</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>352612</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1">
+        <v>43085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filter date attempt 32
</commit_message>
<xml_diff>
--- a/Data/DataSheet.xlsx
+++ b/Data/DataSheet.xlsx
@@ -371,9 +371,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>